<commit_message>
modified code to use port expander for most digital signals
</commit_message>
<xml_diff>
--- a/Arduino_tuner/Arduino tuner.xlsx
+++ b/Arduino_tuner/Arduino tuner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\Arduino_tuner\Arduino_tuner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A67E653-4CB9-45FA-8E0F-48F48A2263BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C70BCF-8271-42D6-9B7F-6A623285DD26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15460" xr2:uid="{C8983B7A-4E70-4BE1-B148-993DE7EEEC3C}"/>
+    <workbookView xWindow="2410" yWindow="2070" windowWidth="28800" windowHeight="15460" xr2:uid="{C8983B7A-4E70-4BE1-B148-993DE7EEEC3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t>Pin name</t>
   </si>
@@ -45,60 +45,24 @@
     <t>wire #</t>
   </si>
   <si>
-    <t>D0</t>
-  </si>
-  <si>
     <t>K1</t>
   </si>
   <si>
     <t>L1</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
     <t>D3</t>
   </si>
   <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>D5</t>
-  </si>
-  <si>
-    <t>D6</t>
-  </si>
-  <si>
     <t>K2</t>
   </si>
   <si>
     <t>L2</t>
   </si>
   <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>D8</t>
-  </si>
-  <si>
-    <t>D9</t>
-  </si>
-  <si>
-    <t>D10</t>
-  </si>
-  <si>
-    <t>D11</t>
-  </si>
-  <si>
-    <t>D12</t>
-  </si>
-  <si>
-    <t>D13</t>
-  </si>
-  <si>
     <t>K3</t>
   </si>
   <si>
@@ -213,15 +177,6 @@
     <t>640 pF</t>
   </si>
   <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
     <t>VCC</t>
   </si>
   <si>
@@ -231,9 +186,6 @@
     <t>K9</t>
   </si>
   <si>
-    <t>Lin/Cin</t>
-  </si>
-  <si>
     <t>Bridge</t>
   </si>
   <si>
@@ -244,14 +196,89 @@
   </si>
   <si>
     <t>gnd plane</t>
+  </si>
+  <si>
+    <t>GPA0</t>
+  </si>
+  <si>
+    <t>GPA1</t>
+  </si>
+  <si>
+    <t>GPA2</t>
+  </si>
+  <si>
+    <t>GPA3</t>
+  </si>
+  <si>
+    <t>GPA4</t>
+  </si>
+  <si>
+    <t>GPA5</t>
+  </si>
+  <si>
+    <t>GPA6</t>
+  </si>
+  <si>
+    <t>GPA7</t>
+  </si>
+  <si>
+    <r>
+      <t>GP</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>B0</t>
+    </r>
+  </si>
+  <si>
+    <t>GPB1</t>
+  </si>
+  <si>
+    <t>GPB2</t>
+  </si>
+  <si>
+    <t>GPB3</t>
+  </si>
+  <si>
+    <t>GPB4</t>
+  </si>
+  <si>
+    <t>GPB5</t>
+  </si>
+  <si>
+    <t>GPB6</t>
+  </si>
+  <si>
+    <t>GPB7</t>
+  </si>
+  <si>
+    <t>Tune button</t>
+  </si>
+  <si>
+    <t>Cin/Cout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -279,9 +306,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -598,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7FD1EB-CC68-4B7F-A29F-3C14F2E446EF}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -636,19 +666,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1">
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -656,19 +686,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
@@ -676,19 +706,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1">
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
@@ -696,19 +726,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1">
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="F5" s="1">
         <v>4</v>
@@ -716,19 +746,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="B6" s="1">
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="F6" s="1">
         <v>5</v>
@@ -736,19 +766,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="B7" s="1">
         <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="F7" s="1">
         <v>6</v>
@@ -756,19 +786,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="F8" s="1">
         <v>7</v>
@@ -776,19 +806,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1">
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F10" s="1">
         <v>8</v>
@@ -796,39 +826,39 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1">
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F11" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>19</v>
+      <c r="A12" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="B12" s="1">
         <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F12" s="1">
         <v>10</v>
@@ -836,19 +866,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="B13" s="1">
         <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F13" s="1">
         <v>11</v>
@@ -856,19 +886,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="B14" s="1">
         <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F14" s="1">
         <v>12</v>
@@ -876,19 +906,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="B15" s="1">
         <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="F15" s="1">
         <v>13</v>
@@ -896,19 +926,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="B16" s="1">
         <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F16" s="1">
         <v>14</v>
@@ -916,16 +946,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1">
         <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F18" s="1">
         <v>15</v>
@@ -933,65 +963,73 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B19" s="1">
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="F19" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="1">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1">
         <v>4</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="1">
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="1">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="1">
-        <v>18</v>
-      </c>
-      <c r="F22" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" s="1">
-        <v>8</v>
-      </c>
-      <c r="F23" s="1">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>72</v>
+        <v>50</v>
+      </c>
+      <c r="B24" s="1">
+        <v>18</v>
       </c>
       <c r="F24" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="1">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="1">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed swr display, added code for tune button
</commit_message>
<xml_diff>
--- a/Arduino_tuner/Arduino tuner.xlsx
+++ b/Arduino_tuner/Arduino tuner.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\Arduino_tuner\Arduino_tuner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C70BCF-8271-42D6-9B7F-6A623285DD26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72BB9A7-5AE0-450C-AF25-12C3F4DF8023}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2410" yWindow="2070" windowWidth="28800" windowHeight="15460" xr2:uid="{C8983B7A-4E70-4BE1-B148-993DE7EEEC3C}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15460" xr2:uid="{C8983B7A-4E70-4BE1-B148-993DE7EEEC3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>Pin name</t>
   </si>
@@ -222,22 +222,6 @@
     <t>GPA7</t>
   </si>
   <si>
-    <r>
-      <t>GP</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>B0</t>
-    </r>
-  </si>
-  <si>
     <t>GPB1</t>
   </si>
   <si>
@@ -263,6 +247,15 @@
   </si>
   <si>
     <t>Cin/Cout</t>
+  </si>
+  <si>
+    <t>GPB0</t>
+  </si>
+  <si>
+    <t>Switch NO</t>
+  </si>
+  <si>
+    <t>active low</t>
   </si>
 </sst>
 </file>
@@ -628,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7FD1EB-CC68-4B7F-A29F-3C14F2E446EF}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -644,7 +637,7 @@
     <col min="6" max="6" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,8 +656,9 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
@@ -684,9 +678,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1">
         <v>12</v>
@@ -704,9 +698,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1">
         <v>13</v>
@@ -724,9 +718,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B5" s="1">
         <v>14</v>
@@ -744,9 +738,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1">
         <v>15</v>
@@ -764,9 +758,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B7" s="1">
         <v>16</v>
@@ -784,9 +778,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -804,9 +798,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1">
         <v>22</v>
@@ -824,9 +818,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1">
         <v>23</v>
@@ -844,9 +838,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B12" s="1">
         <v>24</v>
@@ -864,9 +858,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1">
         <v>25</v>
@@ -884,9 +878,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B14" s="1">
         <v>26</v>
@@ -904,9 +898,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B15" s="1">
         <v>27</v>
@@ -924,7 +918,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>70</v>
       </c>
@@ -944,9 +938,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1">
         <v>9</v>
@@ -955,15 +949,15 @@
         <v>52</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F18" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" s="1">
         <v>6</v>
@@ -978,7 +972,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -992,15 +986,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B22" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="E22" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+      <c r="G22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
refactored so mapping is unabiguous, tested
</commit_message>
<xml_diff>
--- a/Arduino_tuner/Arduino tuner.xlsx
+++ b/Arduino_tuner/Arduino tuner.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\Arduino_tuner\Arduino_tuner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86156173-102C-4D48-8CDD-411DD683D98E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAED6248-9C99-40EE-B8FD-BA6EA2D4C380}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15460" xr2:uid="{C8983B7A-4E70-4BE1-B148-993DE7EEEC3C}"/>
+    <workbookView xWindow="6310" yWindow="3780" windowWidth="28800" windowHeight="15460" xr2:uid="{C8983B7A-4E70-4BE1-B148-993DE7EEEC3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
   <si>
     <t>Pin name</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>active low</t>
+  </si>
+  <si>
+    <t>Pin ID</t>
   </si>
 </sst>
 </file>
@@ -621,24 +624,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7FD1EB-CC68-4B7F-A29F-3C14F2E446EF}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -646,391 +650,448 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="1">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B3" s="1">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B4" s="1">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B5" s="1">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="1">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B6" s="1">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B7" s="1">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="1">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="1">
         <v>22</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="1">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B11" s="1">
         <v>23</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="1">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="1">
         <v>24</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="1">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="1">
         <v>25</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="1">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B14" s="1">
         <v>26</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="1">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B15" s="1">
         <v>27</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="1">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B16" s="1">
         <v>28</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="1">
+        <v>14</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B18" s="1">
         <v>9</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="1">
+        <v>7</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B19" s="1">
         <v>6</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="1">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="1">
         <v>4</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="1">
         <v>18</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B25" s="1">
         <v>8</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>20</v>
       </c>
     </row>

</xml_diff>